<commit_message>
finalizando analise estatistica descritiva e iniciando inferencial/chi etc
</commit_message>
<xml_diff>
--- a/Tabelas de Saída.xlsx
+++ b/Tabelas de Saída.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="161">
   <si>
     <t>Estado civil</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>Porcentagem (Desconhecido)</t>
+  </si>
+  <si>
+    <t>Cor</t>
   </si>
 </sst>
 </file>
@@ -882,42 +885,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>31</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>79.48999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>20.51</v>
       </c>
     </row>
@@ -928,75 +937,90 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>53.85</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>30.77</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>7.69</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>5.13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>2.56</v>
       </c>
     </row>
@@ -1007,75 +1031,90 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>46.15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>30.77</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15.38</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>5.13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>2.56</v>
       </c>
     </row>
@@ -1086,53 +1125,62 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>33</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>84.62</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>12.82</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>2.56</v>
       </c>
     </row>
@@ -1143,42 +1191,48 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>28</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>71.79000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>28.21</v>
       </c>
     </row>
@@ -1189,108 +1243,132 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>43.59</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>30.77</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>10.26</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>5.13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
       <c r="C6">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
       <c r="C7">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
       <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>2.56</v>
       </c>
     </row>
@@ -1301,119 +1379,146 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>43.59</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>28.21</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>12.82</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
       <c r="C6">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
       <c r="C7">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
       <c r="C9">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
       <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>2.56</v>
       </c>
     </row>
@@ -1424,42 +1529,48 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>38</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>97.44</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2.56</v>
       </c>
     </row>
@@ -1470,42 +1581,48 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>56.41</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>43.59</v>
       </c>
     </row>
@@ -1516,42 +1633,48 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>56.41</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>43.59</v>
       </c>
     </row>
@@ -1562,42 +1685,48 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>53.85</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>46.15</v>
       </c>
     </row>
@@ -1608,42 +1737,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>59.46</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>40.54</v>
       </c>
     </row>
@@ -1654,119 +1789,146 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>38</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>97.44</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>5.13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>61</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
       <c r="C7">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>28.21</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
       <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>2.56</v>
       </c>
     </row>
@@ -1777,86 +1939,104 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>36</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>92.31</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>5.13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>5.13</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>5.13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>25.64</v>
       </c>
     </row>
@@ -1867,42 +2047,48 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>37</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>94.87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>5.13</v>
       </c>
     </row>
@@ -1913,42 +2099,48 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>30</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>76.92</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>23.08</v>
       </c>
     </row>
@@ -1959,31 +2151,34 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>39</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>100</v>
       </c>
     </row>
@@ -1994,163 +2189,202 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>33.33</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>74</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>38.46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>22</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>56.41</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>35.9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>77</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>22</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>56.41</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>78</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>34</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>87.18000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>79</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>24</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>61.54</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>80</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>29</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>74.36</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>81</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>26</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>66.67</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>82</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>21</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>53.85</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>83</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>32</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>82.05</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>84</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>30.77</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>85</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>30</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>76.92</v>
       </c>
     </row>
@@ -2161,119 +2395,146 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>23.08</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>33.33</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>25.64</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>15.38</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
       <c r="C6">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>25.64</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>93</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>15.38</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>94</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>33.33</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>95</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>12.82</v>
       </c>
     </row>
@@ -2284,64 +2545,76 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>20.51</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>98</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>33.33</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>99</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>33</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>84.62</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>100</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>23.08</v>
       </c>
     </row>
@@ -2352,42 +2625,48 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>37</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>94.87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>5.13</v>
       </c>
     </row>
@@ -2398,31 +2677,34 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>39</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>100</v>
       </c>
     </row>
@@ -2433,64 +2715,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>51.28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>23.08</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>17.95</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>7.69</v>
       </c>
     </row>
@@ -2501,251 +2795,314 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>104</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>15</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>38.46</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>105</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>5.13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>5.13</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>5.13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>5.13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>107</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
       <c r="C7">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>108</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>109</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
       <c r="C9">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>110</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
       <c r="C10">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>111</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
       <c r="C11">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>112</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
       <c r="C12">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>113</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
       <c r="C13">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>114</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
       <c r="C14">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
       <c r="C15">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
       <c r="C16">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
       <c r="C17">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
       <c r="C18">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>115</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
       <c r="C19">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>116</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
       <c r="C20">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>117</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
       <c r="C21">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>118</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>2.56</v>
       </c>
     </row>
@@ -2756,416 +3113,524 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>120</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>122</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>123</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>10.26</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>125</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
       <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>5.13</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>126</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>7.69</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>127</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
       <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>5.13</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>128</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
       <c r="C10">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>129</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
       <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>5.13</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>130</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
       <c r="C12">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>131</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
       <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
         <v>5.13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>132</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>6</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>15.38</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>133</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
       <c r="C15">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>134</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>9</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>23.08</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>135</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
       <c r="C17">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>136</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
       <c r="C18">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>137</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
       <c r="C19">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>138</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
       <c r="C20">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>139</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
       <c r="C21">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>140</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>3</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>7.69</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>141</v>
       </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
       <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
         <v>5.13</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>142</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
       <c r="C24">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>143</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>3</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>7.69</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>144</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
       <c r="C26">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>145</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>13</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>33.33</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>146</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
       <c r="C28">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>147</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
       <c r="C29">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>148</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
       <c r="C30">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>149</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
       <c r="C31">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>150</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>4</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>10.26</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>151</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
       <c r="C33">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>152</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
       <c r="C34">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
         <v>153</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
       <c r="C35">
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>154</v>
       </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
       <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
         <v>5.13</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>155</v>
       </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
       <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
         <v>5.13</v>
       </c>
     </row>
@@ -3176,239 +3641,269 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>2</v>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>13.33</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>26.09</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>0</v>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>13</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>13</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>56.52</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>33.33</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>17.39</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2</v>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>13.33</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>13.04</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>0</v>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>4.35</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>60</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>6</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>33.33</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>20</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>39.13</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>1</v>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>6.67</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>13.04</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>100</v>
       </c>
     </row>
@@ -3419,53 +3914,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>23</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>58.97</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>38.46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>2.56</v>
       </c>
     </row>
@@ -3476,42 +3980,48 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>35</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>89.73999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>10.26</v>
       </c>
     </row>
@@ -3522,42 +4032,48 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>32</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>82.05</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>17.95</v>
       </c>
     </row>
@@ -3568,50 +4084,59 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>7.51</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3">
-        <v>26</v>
       </c>
       <c r="C3">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="D3">
         <v>26</v>
       </c>
-      <c r="B4">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>13</v>
       </c>
     </row>
@@ -3622,42 +4147,48 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>30</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>76.92</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>23.08</v>
       </c>
     </row>
@@ -3668,42 +4199,48 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>37</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>94.87</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>5.13</v>
       </c>
     </row>

</xml_diff>